<commit_message>
Avance muestreo de datos
</commit_message>
<xml_diff>
--- a/SpaOnline/Fabricante - Muestreo Datos.xlsx
+++ b/SpaOnline/Fabricante - Muestreo Datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/SpaOnline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CEC2781-028A-4B20-B688-2C0F59641A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF11142-363C-4382-BBF4-DB412622E24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
@@ -103,7 +103,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,12 +126,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -589,7 +583,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,13 +598,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -655,12 +651,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>